<commit_message>
test and fix: get_title_keyword, get_post_data
</commit_message>
<xml_diff>
--- a/data/news_and_keyword/kosdaq/3S.xlsx
+++ b/data/news_and_keyword/kosdaq/3S.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1297,994 +1297,6 @@
         <v>12.61261261261261</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2015-05-27 09:50:00</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>약세…작년 적자폭 확대</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>['적자폭', '확대']</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E34" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F34" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2015-05-27 09:27:00</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>지난해 실적 악화 소식에 하락</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>['지난해', '실적', '악화', '소식에', '하락']</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E35" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F35" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2014-05-14 11:12:00</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>적자전환 소식에 7%대 급락</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>['적자전환', '소식에', '7', '대', '급락']</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E36" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F36" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2014-05-14 10:20:00</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>코리아, 적자 전환 '급락'</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>['코리아', '적자', '전환']</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E37" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F37" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2014-05-14 10:15:00</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>지난해 실적 부진으로 주가 ↓</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>['지난해', '실적', '부진으로', '주가']</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E38" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F38" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2014-05-14 09:47:00</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>코리아, 적자전환 소식에 급락</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>['코리아', '적자전환', '소식에', '급락']</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E39" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F39" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2014-05-14 09:34:00</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>코리아, 지난해 실적 부진…약세</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>['코리아', '지난해', '실적']</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E40" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F40" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2014-05-14 09:31:00</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>작년 적자전환에 하락</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>['작년', '적자전환에', '하락']</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E41" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F41" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2014-05-14 09:10:00</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>약세…지난해 영업익·순익 적자전환</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>['적자전환']</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E42" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F42" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2014-04-22 10:56:00</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>너무 빠졌나…사흘만에 반등</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>['너무', '반등']</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E43" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F43" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2014-03-07 10:57:00</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>실적 기대감에 강세…안성2공장 매출증대 '기대'</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>['실적', '기대감에', '매출증대']</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E44" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F44" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2013-12-26 09:39:00</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>8일만에 반등… 실적 기대감에 강세</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>['8일만에', '실적', '기대감에', '강세']</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E45" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F45" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>2012-09-27 09:23:00</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>바닥 쳤나… 이틀째 上</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>['바닥', '이틀째', '上']</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E46" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F46" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>2012-09-26 10:27:00</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>급락 제동, 하락 5일만에 장중 上</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>['급락', '제동', '하락', '5일만에', '장중']</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E47" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F47" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>2012-09-26 09:52:00</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>저가 매수세…6일 만에 상한가</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>['저가', '만에', '상한가']</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E48" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F48" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>2012-02-23 09:17:00</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>대규모 유증에도 급등세</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>['대규모', '유증에도', '급등세']</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E49" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F49" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>2011-12-09 14:43:00</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>또다시 이상급등…3일 연속 ↑</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>['또다시', '연속']</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E50" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F50" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>2011-12-09 10:08:00</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>하락장서 강세.. 4%대↑</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>['하락장서', '강세', '4']</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E51" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F51" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>2011-12-07 09:30:00</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>투자경고 해제된 날 하락 반전</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>['투자경고', '해제된', '날', '하락', '반전']</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E52" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F52" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>2011-11-28 09:46:00</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>나흘째 급락세</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>['나흘째', '급락세']</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E53" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F53" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>2011-11-24 09:36:00</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>이틀 하한가..시총순위 12→21위</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>['이틀', '하한가', '시총순위']</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E54" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F54" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>2011-11-24 09:25:00</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>투자경고 종목 지정에 연일 급락</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>['투자경고', '종목', '지정에', '연일', '급락']</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E55" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F55" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>2011-11-23 10:28:00</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>하한가…PER 100배, 지나치다</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>['100배', '지나치다']</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E56" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F56" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>2011-11-23 10:05:00</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>투자경고 종목 지정에 하한가 추락</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>['투자경고', '종목', '지정에', '하한가', '추락']</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E57" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F57" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>2011-11-23 09:47:00</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>묻지마 급등 `그만`..하한가로 추락</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>['묻지마', '급등', '그만', '하한가로', '추락']</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E58" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F58" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>2011-11-23 09:31:00</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>투자경고종목 지정.. 급등 14일만에 '하한'</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>['투자경고종목', '지정', '급등', '14일만에']</t>
-        </is>
-      </c>
-      <c r="D59" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E59" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F59" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>2011-11-23 09:30:00</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>'묻지마 강세' 끝내고 급락</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>['강세', '끝내고', '급락']</t>
-        </is>
-      </c>
-      <c r="D60" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E60" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F60" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>2011-11-23 09:19:00</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>14거래일만에 이상급등 마감..'급락'</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>['14거래일만에', '이상급등', '마감']</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E61" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F61" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>2011-11-22 09:25:00</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>이상급등세… 13거래일째 랠리</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>['13거래일째', '랠리']</t>
-        </is>
-      </c>
-      <c r="D62" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E62" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F62" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>2011-11-22 09:11:00</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>'이상급등' 13거래일째..9%↑</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>['13거래일째', '9']</t>
-        </is>
-      </c>
-      <c r="D63" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E63" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F63" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>2011-11-21 09:34:00</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>'이유없이' 12일째 급등? 어느새 시총 13위</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>['12일째', '급등', '어느새', '시총', '13위']</t>
-        </is>
-      </c>
-      <c r="D64" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E64" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F64" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>2011-11-21 09:18:00</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>12거래일째 상승랠리</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>['12거래일째', '상승랠리']</t>
-        </is>
-      </c>
-      <c r="D65" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E65" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F65" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>2010-04-22 11:50:00</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>전방산업 수혜...52주 신고가 갱신</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>['전방산업', '수혜', '52주', '신고가', '갱신']</t>
-        </is>
-      </c>
-      <c r="D66" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E66" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F66" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>2009-04-09 10:40:00</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>실적 기대 반영? 사흘째 급등</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>['실적', '기대', '반영', '사흘째', '급등']</t>
-        </is>
-      </c>
-      <c r="D67" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E67" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F67" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>2009-04-08 14:34:00</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>코리아, 신규사업 기대감 이틀째 상한가</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>['코리아', '신규사업', '기대감', '이틀째', '상한가']</t>
-        </is>
-      </c>
-      <c r="D68" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E68" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F68" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>2008-09-11 14:54:00</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>日협력사 지분투자 기대감으로 강세</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>['日협력사', '지분투자', '기대감으로', '강세']</t>
-        </is>
-      </c>
-      <c r="D69" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E69" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F69" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>2006-12-11 09:10:00</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>대규모 유증결의..하락</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>['대규모', '유증결의', '하락']</t>
-        </is>
-      </c>
-      <c r="D70" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E70" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F70" t="n">
-        <v>-400</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>2005-07-20 09:24:00</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>적조 소식에 '상한가'</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>['적조', '소식에']</t>
-        </is>
-      </c>
-      <c r="D71" t="n">
-        <v>-400</v>
-      </c>
-      <c r="E71" t="n">
-        <v>-400</v>
-      </c>
-      <c r="F71" t="n">
-        <v>-400</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>